<commit_message>
Refactoring UI to use fragments
</commit_message>
<xml_diff>
--- a/docs/planning.xlsx
+++ b/docs/planning.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colin\Documents\src\GwentSite\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colin.monroe\Documents\Github\GwentSite\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>User</t>
   </si>
@@ -63,12 +63,18 @@
   </si>
   <si>
     <t>Filter Screen (coll?)</t>
+  </si>
+  <si>
+    <t>Start Page (dashboard)</t>
+  </si>
+  <si>
+    <t>Card Viewer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -207,6 +213,203 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1514475</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2828925" y="1114425"/>
+          <a:ext cx="1047750" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2133600" y="1181100"/>
+          <a:ext cx="0" cy="485775"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2133600" y="428625"/>
+          <a:ext cx="0" cy="523875"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4191000" y="1162050"/>
+          <a:ext cx="0" cy="1295400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -506,103 +709,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G14"/>
+  <dimension ref="B2:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="57.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="7" t="s">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>